<commit_message>
Update Masters Madrid Players.xlsx
</commit_message>
<xml_diff>
--- a/Masters Madrid Players.xlsx
+++ b/Masters Madrid Players.xlsx
@@ -694,7 +694,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
   <si>
     <t>Country</t>
   </si>
@@ -705,12 +705,15 @@
     <t>Player</t>
   </si>
   <si>
-    <t>Tournaments</t>
+    <t>Tournaments Attended (34)</t>
   </si>
   <si>
     <t>Highest Placed</t>
   </si>
   <si>
+    <t>Tournaments Attended (5)</t>
+  </si>
+  <si>
     <t>zekken</t>
   </si>
   <si>
@@ -723,6 +726,72 @@
     <t>9th - 16th</t>
   </si>
   <si>
+    <t>Sacy</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>Magnum</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>TenZ</t>
+  </si>
+  <si>
+    <t>marteen</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>johnqt</t>
+  </si>
+  <si>
+    <t>N4RRATE</t>
+  </si>
+  <si>
+    <t>Zellsis</t>
+  </si>
+  <si>
+    <t>tomaszy</t>
+  </si>
+  <si>
+    <t>Less</t>
+  </si>
+  <si>
+    <t>Boo</t>
+  </si>
+  <si>
+    <t>17th - 32nd</t>
+  </si>
+  <si>
+    <t>Saadhak</t>
+  </si>
+  <si>
+    <t>benjyfishy</t>
+  </si>
+  <si>
+    <t>cauanzin</t>
+  </si>
+  <si>
+    <t>MiniBoo</t>
+  </si>
+  <si>
+    <t>tuyz</t>
+  </si>
+  <si>
+    <t>RieNs</t>
+  </si>
+  <si>
+    <t>qck</t>
+  </si>
+  <si>
+    <t>paTiTek</t>
+  </si>
+  <si>
     <t>Meteor</t>
   </si>
   <si>
@@ -732,36 +801,12 @@
     <t>Haodong</t>
   </si>
   <si>
-    <t>Sacy</t>
-  </si>
-  <si>
-    <t>1st</t>
-  </si>
-  <si>
-    <t>Magnum</t>
-  </si>
-  <si>
-    <t>2nd</t>
-  </si>
-  <si>
     <t>t3xture</t>
   </si>
   <si>
-    <t>17th - 32nd</t>
-  </si>
-  <si>
     <t>CHICHOO</t>
   </si>
   <si>
-    <t>TenZ</t>
-  </si>
-  <si>
-    <t>marteen</t>
-  </si>
-  <si>
-    <t>NaN</t>
-  </si>
-  <si>
     <t>Lakia</t>
   </si>
   <si>
@@ -771,36 +816,18 @@
     <t>nobody</t>
   </si>
   <si>
-    <t>johnqt</t>
-  </si>
-  <si>
-    <t>N4RRATE</t>
-  </si>
-  <si>
     <t>Munchkin</t>
   </si>
   <si>
     <t>ZmjjKK</t>
   </si>
   <si>
-    <t>Zellsis</t>
-  </si>
-  <si>
-    <t>tomaszy</t>
-  </si>
-  <si>
     <t>Karon</t>
   </si>
   <si>
     <t>Smoggy</t>
   </si>
   <si>
-    <t>Less</t>
-  </si>
-  <si>
-    <t>Boo</t>
-  </si>
-  <si>
     <t>mindfreak</t>
   </si>
   <si>
@@ -810,36 +837,18 @@
     <t>13th - 16th</t>
   </si>
   <si>
-    <t>Saadhak</t>
-  </si>
-  <si>
-    <t>benjyfishy</t>
-  </si>
-  <si>
     <t>f0rsakeN</t>
   </si>
   <si>
     <t>BerLIN</t>
   </si>
   <si>
-    <t>cauanzin</t>
-  </si>
-  <si>
-    <t>MiniBoo</t>
-  </si>
-  <si>
     <t>d4v41</t>
   </si>
   <si>
     <t>Lysoar</t>
   </si>
   <si>
-    <t>tuyz</t>
-  </si>
-  <si>
-    <t>RieNs</t>
-  </si>
-  <si>
     <t>something</t>
   </si>
   <si>
@@ -850,12 +859,6 @@
   </si>
   <si>
     <t>NaN (5th - 8th)</t>
-  </si>
-  <si>
-    <t>qck</t>
-  </si>
-  <si>
-    <t>paTiTek</t>
   </si>
   <si>
     <t>Monyet</t>
@@ -877,10 +880,18 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1053,12 +1064,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.15"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1182,12 +1199,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1206,12 +1217,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1277,7 +1282,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1295,7 +1300,85 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -1418,55 +1501,52 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1481,102 +1561,165 @@
     <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1853,6 +1996,13 @@
       <tableStyleElement type="pageFieldValues" dxfId="8"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="00FF570C"/>
+      <color rgb="0001D2D7"/>
+      <color rgb="00E73056"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2119,37 +2269,37 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.61904761904762" customWidth="1"/>
-    <col min="2" max="2" width="6.42857142857143" customWidth="1"/>
-    <col min="3" max="3" width="9.28571428571429" customWidth="1"/>
-    <col min="4" max="4" width="13.7142857142857" customWidth="1"/>
-    <col min="5" max="5" width="15.1428571428571" customWidth="1"/>
-    <col min="6" max="6" width="8.6" customWidth="1"/>
-    <col min="7" max="7" width="6.42857142857143" customWidth="1"/>
-    <col min="8" max="8" width="9.28571428571429" customWidth="1"/>
-    <col min="9" max="9" width="13.7142857142857" customWidth="1"/>
-    <col min="10" max="10" width="15.1428571428571" customWidth="1"/>
-    <col min="11" max="11" width="8.57142857142857" customWidth="1"/>
-    <col min="12" max="12" width="6.42857142857143" customWidth="1"/>
-    <col min="13" max="13" width="10.2857142857143" customWidth="1"/>
-    <col min="14" max="14" width="13.7142857142857" customWidth="1"/>
-    <col min="15" max="15" width="15.1428571428571" customWidth="1"/>
-    <col min="16" max="16" width="8.57142857142857" customWidth="1"/>
-    <col min="17" max="17" width="6.42857142857143" customWidth="1"/>
-    <col min="18" max="18" width="9.28571428571429" customWidth="1"/>
-    <col min="19" max="19" width="13.7142857142857" customWidth="1"/>
-    <col min="20" max="20" width="15.1428571428571" customWidth="1"/>
+    <col min="1" max="1" width="9.42857142857143" customWidth="1"/>
+    <col min="2" max="2" width="6.85714285714286" customWidth="1"/>
+    <col min="3" max="3" width="11.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="16.5714285714286" customWidth="1"/>
+    <col min="6" max="6" width="10.0380952380952" customWidth="1"/>
+    <col min="7" max="7" width="6.99047619047619" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="29.7142857142857" customWidth="1"/>
+    <col min="10" max="10" width="16.5714285714286" customWidth="1"/>
+    <col min="11" max="11" width="9.42857142857143" customWidth="1"/>
+    <col min="12" max="12" width="6.85714285714286" customWidth="1"/>
+    <col min="13" max="13" width="11.1428571428571" customWidth="1"/>
+    <col min="14" max="14" width="31" customWidth="1"/>
+    <col min="15" max="15" width="16.5714285714286" customWidth="1"/>
+    <col min="16" max="16" width="9.42857142857143" customWidth="1"/>
+    <col min="17" max="17" width="6.85714285714286" customWidth="1"/>
+    <col min="18" max="18" width="9.85714285714286" customWidth="1"/>
+    <col min="19" max="19" width="31" customWidth="1"/>
+    <col min="20" max="20" width="16.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" ht="16.5" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2175,906 +2325,1136 @@
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
     </row>
     <row r="2" ht="31" customHeight="1" spans="1:20">
-      <c r="A2" s="1" t="str">
+      <c r="A2" s="2" t="str">
         <f>_xlfn.DISPIMG("ID_BA2487D371F2480A955BB261416FB890",1)</f>
         <v>=DISPIMG("ID_BA2487D371F2480A955BB261416FB890",1)</v>
       </c>
-      <c r="B2" s="1" t="str">
+      <c r="B2" s="3" t="str">
         <f>_xlfn.DISPIMG("ID_0DCABE9F44DA4E239F21ECDEB726BF58",1)</f>
         <v>=DISPIMG("ID_0DCABE9F44DA4E239F21ECDEB726BF58",1)</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="str">
+      <c r="E2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="str">
         <f>_xlfn.DISPIMG("ID_054258D69663499AADA6A9FCA4E10F45",1)</f>
         <v>=DISPIMG("ID_054258D69663499AADA6A9FCA4E10F45",1)</v>
       </c>
-      <c r="G2" s="1" t="str">
+      <c r="G2" s="3" t="str">
         <f>_xlfn.DISPIMG("ID_7E54EC765F954BF0BF6E3014289FAE84",1)</f>
         <v>=DISPIMG("ID_7E54EC765F954BF0BF6E3014289FAE84",1)</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="5">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="25"/>
+    </row>
+    <row r="3" ht="31" customHeight="1" spans="1:20">
+      <c r="A3" s="7" t="str">
+        <f>_xlfn.DISPIMG("ID_268B8A0A44544341B29F9DDA7FA1D51C",1)</f>
+        <v>=DISPIMG("ID_268B8A0A44544341B29F9DDA7FA1D51C",1)</v>
+      </c>
+      <c r="B3" s="8" t="str">
+        <f>_xlfn.DISPIMG("ID_0DCABE9F44DA4E239F21ECDEB726BF58",1)</f>
+        <v>=DISPIMG("ID_0DCABE9F44DA4E239F21ECDEB726BF58",1)</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="10">
+        <v>4</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="7" t="str">
+        <f>_xlfn.DISPIMG("ID_57DECDAF621B4ABDBC7D8E64B2E10BEC",1)</f>
+        <v>=DISPIMG("ID_57DECDAF621B4ABDBC7D8E64B2E10BEC",1)</v>
+      </c>
+      <c r="G3" s="8" t="str">
+        <f>_xlfn.DISPIMG("ID_7E54EC765F954BF0BF6E3014289FAE84",1)</f>
+        <v>=DISPIMG("ID_7E54EC765F954BF0BF6E3014289FAE84",1)</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="10">
+        <v>3</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="25"/>
+    </row>
+    <row r="4" ht="31" customHeight="1" spans="1:20">
+      <c r="A4" s="7" t="str">
+        <f>_xlfn.DISPIMG("ID_7BE895EBAF304A60A4C5B4F2F664E2C4",1)</f>
+        <v>=DISPIMG("ID_7BE895EBAF304A60A4C5B4F2F664E2C4",1)</v>
+      </c>
+      <c r="B4" s="8" t="str">
+        <f>_xlfn.DISPIMG("ID_0DCABE9F44DA4E239F21ECDEB726BF58",1)</f>
+        <v>=DISPIMG("ID_0DCABE9F44DA4E239F21ECDEB726BF58",1)</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="10">
+        <v>3</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="7" t="str">
+        <f>_xlfn.DISPIMG("ID_57DECDAF621B4ABDBC7D8E64B2E10BEC",1)</f>
+        <v>=DISPIMG("ID_57DECDAF621B4ABDBC7D8E64B2E10BEC",1)</v>
+      </c>
+      <c r="G4" s="8" t="str">
+        <f>_xlfn.DISPIMG("ID_7E54EC765F954BF0BF6E3014289FAE84",1)</f>
+        <v>=DISPIMG("ID_7E54EC765F954BF0BF6E3014289FAE84",1)</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="10">
+        <v>0</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="25"/>
+    </row>
+    <row r="5" ht="31" customHeight="1" spans="1:20">
+      <c r="A5" s="7" t="str">
+        <f>_xlfn.DISPIMG("ID_F2534797B2514259B37B3F90C14104CE",1)</f>
+        <v>=DISPIMG("ID_F2534797B2514259B37B3F90C14104CE",1)</v>
+      </c>
+      <c r="B5" s="8" t="str">
+        <f>_xlfn.DISPIMG("ID_0DCABE9F44DA4E239F21ECDEB726BF58",1)</f>
+        <v>=DISPIMG("ID_0DCABE9F44DA4E239F21ECDEB726BF58",1)</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="7" t="str">
+        <f>_xlfn.DISPIMG("ID_BA2487D371F2480A955BB261416FB890",1)</f>
+        <v>=DISPIMG("ID_BA2487D371F2480A955BB261416FB890",1)</v>
+      </c>
+      <c r="G5" s="8" t="str">
+        <f>_xlfn.DISPIMG("ID_7E54EC765F954BF0BF6E3014289FAE84",1)</f>
+        <v>=DISPIMG("ID_7E54EC765F954BF0BF6E3014289FAE84",1)</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="25"/>
+    </row>
+    <row r="6" ht="31" customHeight="1" spans="1:20">
+      <c r="A6" s="7" t="str">
+        <f>_xlfn.DISPIMG("ID_BA2487D371F2480A955BB261416FB890",1)</f>
+        <v>=DISPIMG("ID_BA2487D371F2480A955BB261416FB890",1)</v>
+      </c>
+      <c r="B6" s="8" t="str">
+        <f>_xlfn.DISPIMG("ID_0DCABE9F44DA4E239F21ECDEB726BF58",1)</f>
+        <v>=DISPIMG("ID_0DCABE9F44DA4E239F21ECDEB726BF58",1)</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="10">
+        <v>2</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="3">
+      <c r="F6" s="7" t="str">
+        <f>_xlfn.DISPIMG("ID_9A490142D9BF4C41BEA4AF01A76599D2",1)</f>
+        <v>=DISPIMG("ID_9A490142D9BF4C41BEA4AF01A76599D2",1)</v>
+      </c>
+      <c r="G6" s="8" t="str">
+        <f>_xlfn.DISPIMG("ID_7E54EC765F954BF0BF6E3014289FAE84",1)</f>
+        <v>=DISPIMG("ID_7E54EC765F954BF0BF6E3014289FAE84",1)</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="25"/>
+    </row>
+    <row r="7" ht="31" customHeight="1" spans="1:20">
+      <c r="A7" s="7" t="str">
+        <f t="shared" ref="A7:A11" si="0">_xlfn.DISPIMG("ID_268B8A0A44544341B29F9DDA7FA1D51C",1)</f>
+        <v>=DISPIMG("ID_268B8A0A44544341B29F9DDA7FA1D51C",1)</v>
+      </c>
+      <c r="B7" s="8" t="str">
+        <f>_xlfn.DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</f>
+        <v>=DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="10">
+        <v>6</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="7" t="str">
+        <f>_xlfn.DISPIMG("ID_ED6C9EB4D46D47A0B011F533288D71BF",1)</f>
+        <v>=DISPIMG("ID_ED6C9EB4D46D47A0B011F533288D71BF",1)</v>
+      </c>
+      <c r="G7" s="8" t="str">
+        <f>_xlfn.DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</f>
+        <v>=DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="10">
         <v>1</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_950575228AB54565B95BE1A8CDDED0CF",1)</f>
+      <c r="J7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="25"/>
+    </row>
+    <row r="8" ht="31" customHeight="1" spans="1:20">
+      <c r="A8" s="7" t="str">
+        <f>_xlfn.DISPIMG("ID_6000619F3E9D44F6AE6CD3C3E56CAD75",1)</f>
+        <v>=DISPIMG("ID_6000619F3E9D44F6AE6CD3C3E56CAD75",1)</v>
+      </c>
+      <c r="B8" s="8" t="str">
+        <f>_xlfn.DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</f>
+        <v>=DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="10">
+        <v>6</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="7" t="str">
+        <f>_xlfn.DISPIMG("ID_58AD4992DB3B48FC91CB1DC9640F186D",1)</f>
+        <v>=DISPIMG("ID_58AD4992DB3B48FC91CB1DC9640F186D",1)</v>
+      </c>
+      <c r="G8" s="8" t="str">
+        <f>_xlfn.DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</f>
+        <v>=DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="25"/>
+    </row>
+    <row r="9" ht="31" customHeight="1" spans="1:20">
+      <c r="A9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=DISPIMG("ID_268B8A0A44544341B29F9DDA7FA1D51C",1)</v>
+      </c>
+      <c r="B9" s="8" t="str">
+        <f>_xlfn.DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</f>
+        <v>=DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="10">
+        <v>4</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="7" t="str">
+        <f>_xlfn.DISPIMG("ID_ED6C9EB4D46D47A0B011F533288D71BF",1)</f>
+        <v>=DISPIMG("ID_ED6C9EB4D46D47A0B011F533288D71BF",1)</v>
+      </c>
+      <c r="G9" s="8" t="str">
+        <f>_xlfn.DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</f>
+        <v>=DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="25"/>
+    </row>
+    <row r="10" ht="31" customHeight="1" spans="1:20">
+      <c r="A10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>=DISPIMG("ID_268B8A0A44544341B29F9DDA7FA1D51C",1)</v>
+      </c>
+      <c r="B10" s="8" t="str">
+        <f>_xlfn.DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</f>
+        <v>=DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="10">
+        <v>4</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="7" t="str">
+        <f>_xlfn.DISPIMG("ID_959C3ED946B741B495F5F344457CA70A",1)</f>
+        <v>=DISPIMG("ID_959C3ED946B741B495F5F344457CA70A",1)</v>
+      </c>
+      <c r="G10" s="8" t="str">
+        <f>_xlfn.DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</f>
+        <v>=DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="10">
+        <v>0</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="25"/>
+    </row>
+    <row r="11" ht="31" customHeight="1" spans="1:20">
+      <c r="A11" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>=DISPIMG("ID_268B8A0A44544341B29F9DDA7FA1D51C",1)</v>
+      </c>
+      <c r="B11" s="15" t="str">
+        <f>_xlfn.DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</f>
+        <v>=DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="17">
+        <v>3</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="14" t="str">
+        <f>_xlfn.DISPIMG("ID_6BF2B7BDCEC143CB9B923DEF2ED950E0",1)</f>
+        <v>=DISPIMG("ID_6BF2B7BDCEC143CB9B923DEF2ED950E0",1)</v>
+      </c>
+      <c r="G11" s="15" t="str">
+        <f>_xlfn.DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</f>
+        <v>=DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="17">
+        <v>0</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="25"/>
+    </row>
+    <row r="12" ht="31" customHeight="1" spans="1:19">
+      <c r="A12" s="2" t="str">
+        <f t="shared" ref="A12:A16" si="1">_xlfn.DISPIMG("ID_950575228AB54565B95BE1A8CDDED0CF",1)</f>
         <v>=DISPIMG("ID_950575228AB54565B95BE1A8CDDED0CF",1)</v>
       </c>
-      <c r="L2" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_1F0BE2047E2A4BAEAD892BAD47B3B5A6",1)</f>
+      <c r="B12" s="3" t="str">
+        <f t="shared" ref="B12:B16" si="2">_xlfn.DISPIMG("ID_1F0BE2047E2A4BAEAD892BAD47B3B5A6",1)</f>
         <v>=DISPIMG("ID_1F0BE2047E2A4BAEAD892BAD47B3B5A6",1)</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="3">
+      <c r="C12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="5">
         <v>3</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" s="1" t="str">
+      <c r="E12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="2" t="str">
+        <f t="shared" ref="F12:F17" si="3">_xlfn.DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</f>
+        <v>=DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</v>
+      </c>
+      <c r="G12" s="3" t="str">
+        <f t="shared" ref="G12:G16" si="4">_xlfn.DISPIMG("ID_A78947ADD60E4B9AACFCAE779E0114F7",1)</f>
+        <v>=DISPIMG("ID_A78947ADD60E4B9AACFCAE779E0114F7",1)</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="5">
+        <v>4</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N12" s="27"/>
+      <c r="S12" s="27"/>
+    </row>
+    <row r="13" ht="31" customHeight="1" spans="1:10">
+      <c r="A13" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=DISPIMG("ID_950575228AB54565B95BE1A8CDDED0CF",1)</v>
+      </c>
+      <c r="B13" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>=DISPIMG("ID_1F0BE2047E2A4BAEAD892BAD47B3B5A6",1)</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="10">
+        <v>1</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>=DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</v>
+      </c>
+      <c r="G13" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>=DISPIMG("ID_A78947ADD60E4B9AACFCAE779E0114F7",1)</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="10">
+        <v>4</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" ht="31" customHeight="1" spans="1:10">
+      <c r="A14" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=DISPIMG("ID_950575228AB54565B95BE1A8CDDED0CF",1)</v>
+      </c>
+      <c r="B14" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>=DISPIMG("ID_1F0BE2047E2A4BAEAD892BAD47B3B5A6",1)</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="10">
+        <v>3</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>=DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</v>
+      </c>
+      <c r="G14" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>=DISPIMG("ID_A78947ADD60E4B9AACFCAE779E0114F7",1)</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="10">
+        <v>4</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" ht="31" customHeight="1" spans="1:10">
+      <c r="A15" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=DISPIMG("ID_950575228AB54565B95BE1A8CDDED0CF",1)</v>
+      </c>
+      <c r="B15" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>=DISPIMG("ID_1F0BE2047E2A4BAEAD892BAD47B3B5A6",1)</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="10">
+        <v>5</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>=DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</v>
+      </c>
+      <c r="G15" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>=DISPIMG("ID_A78947ADD60E4B9AACFCAE779E0114F7",1)</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" s="10">
+        <v>4</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" ht="31" customHeight="1" spans="1:10">
+      <c r="A16" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>=DISPIMG("ID_950575228AB54565B95BE1A8CDDED0CF",1)</v>
+      </c>
+      <c r="B16" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>=DISPIMG("ID_1F0BE2047E2A4BAEAD892BAD47B3B5A6",1)</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>=DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</v>
+      </c>
+      <c r="G16" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>=DISPIMG("ID_A78947ADD60E4B9AACFCAE779E0114F7",1)</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="10">
+        <v>4</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" ht="36.05" spans="1:10">
+      <c r="A17" s="7" t="str">
+        <f t="shared" ref="A17:A21" si="5">_xlfn.DISPIMG("ID_AE82F2EF4A454B3CBA695725E1E9B708",1)</f>
+        <v>=DISPIMG("ID_AE82F2EF4A454B3CBA695725E1E9B708",1)</v>
+      </c>
+      <c r="B17" s="8" t="str">
+        <f t="shared" ref="B17:B21" si="6">_xlfn.DISPIMG("ID_1A3A7A7BDCEE4A4E81B55D77328F65F8",1)</f>
+        <v>=DISPIMG("ID_1A3A7A7BDCEE4A4E81B55D77328F65F8",1)</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="10">
+        <v>4</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>=DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</v>
+      </c>
+      <c r="G17" s="8" t="str">
+        <f t="shared" ref="G17:G21" si="7">_xlfn.DISPIMG("ID_D7722B57E05447DEBE72C39EE8A9F731",1)</f>
+        <v>=DISPIMG("ID_D7722B57E05447DEBE72C39EE8A9F731",1)</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="10">
+        <v>2</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" ht="36.05" spans="1:10">
+      <c r="A18" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>=DISPIMG("ID_AE82F2EF4A454B3CBA695725E1E9B708",1)</v>
+      </c>
+      <c r="B18" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>=DISPIMG("ID_1A3A7A7BDCEE4A4E81B55D77328F65F8",1)</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="10">
+        <v>4</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="7" t="str">
+        <f>_xlfn.DISPIMG("ID_6FD6430484BB49FE9601020DAB644F5B",1)</f>
+        <v>=DISPIMG("ID_6FD6430484BB49FE9601020DAB644F5B",1)</v>
+      </c>
+      <c r="G18" s="8" t="str">
+        <f t="shared" si="7"/>
+        <v>=DISPIMG("ID_D7722B57E05447DEBE72C39EE8A9F731",1)</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="10">
+        <v>2</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" ht="36.05" spans="1:10">
+      <c r="A19" s="7" t="str">
+        <f>_xlfn.DISPIMG("ID_58917936AC9A4E2E89C66D86230F0730",1)</f>
+        <v>=DISPIMG("ID_58917936AC9A4E2E89C66D86230F0730",1)</v>
+      </c>
+      <c r="B19" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>=DISPIMG("ID_1A3A7A7BDCEE4A4E81B55D77328F65F8",1)</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="10">
+        <v>4</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="7" t="str">
         <f>_xlfn.DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</f>
         <v>=DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</v>
       </c>
-      <c r="Q2" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_A78947ADD60E4B9AACFCAE779E0114F7",1)</f>
-        <v>=DISPIMG("ID_A78947ADD60E4B9AACFCAE779E0114F7",1)</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="S2" s="3">
-        <v>4</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>6</v>
+      <c r="G19" s="8" t="str">
+        <f t="shared" si="7"/>
+        <v>=DISPIMG("ID_D7722B57E05447DEBE72C39EE8A9F731",1)</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" s="10">
+        <v>1</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="3" ht="31" customHeight="1" spans="1:20">
-      <c r="A3" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_268B8A0A44544341B29F9DDA7FA1D51C",1)</f>
-        <v>=DISPIMG("ID_268B8A0A44544341B29F9DDA7FA1D51C",1)</v>
-      </c>
-      <c r="B3" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_0DCABE9F44DA4E239F21ECDEB726BF58",1)</f>
-        <v>=DISPIMG("ID_0DCABE9F44DA4E239F21ECDEB726BF58",1)</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="3">
-        <v>4</v>
-      </c>
-      <c r="E3" s="5" t="s">
+    <row r="20" ht="36.05" spans="1:10">
+      <c r="A20" s="7" t="str">
+        <f>_xlfn.DISPIMG("ID_AE2522B87EF74B1095DD7DEA2A944CB0",1)</f>
+        <v>=DISPIMG("ID_AE2522B87EF74B1095DD7DEA2A944CB0",1)</v>
+      </c>
+      <c r="B20" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>=DISPIMG("ID_1A3A7A7BDCEE4A4E81B55D77328F65F8",1)</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="10">
+        <v>1</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_57DECDAF621B4ABDBC7D8E64B2E10BEC",1)</f>
-        <v>=DISPIMG("ID_57DECDAF621B4ABDBC7D8E64B2E10BEC",1)</v>
-      </c>
-      <c r="G3" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_7E54EC765F954BF0BF6E3014289FAE84",1)</f>
-        <v>=DISPIMG("ID_7E54EC765F954BF0BF6E3014289FAE84",1)</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="3">
-        <v>3</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_950575228AB54565B95BE1A8CDDED0CF",1)</f>
-        <v>=DISPIMG("ID_950575228AB54565B95BE1A8CDDED0CF",1)</v>
-      </c>
-      <c r="L3" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_1F0BE2047E2A4BAEAD892BAD47B3B5A6",1)</f>
-        <v>=DISPIMG("ID_1F0BE2047E2A4BAEAD892BAD47B3B5A6",1)</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="3">
+      <c r="F20" s="7" t="str">
+        <f>_xlfn.DISPIMG("ID_115E27EB0FD249CAB22FFC543F696862",1)</f>
+        <v>=DISPIMG("ID_115E27EB0FD249CAB22FFC543F696862",1)</v>
+      </c>
+      <c r="G20" s="8" t="str">
+        <f t="shared" si="7"/>
+        <v>=DISPIMG("ID_D7722B57E05447DEBE72C39EE8A9F731",1)</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" ht="36.8" spans="1:10">
+      <c r="A21" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v>=DISPIMG("ID_AE82F2EF4A454B3CBA695725E1E9B708",1)</v>
+      </c>
+      <c r="B21" s="15" t="str">
+        <f t="shared" si="6"/>
+        <v>=DISPIMG("ID_1A3A7A7BDCEE4A4E81B55D77328F65F8",1)</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="17">
         <v>1</v>
       </c>
-      <c r="O3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" s="1" t="str">
+      <c r="E21" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="14" t="str">
         <f>_xlfn.DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</f>
         <v>=DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</v>
       </c>
-      <c r="Q3" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_A78947ADD60E4B9AACFCAE779E0114F7",1)</f>
-        <v>=DISPIMG("ID_A78947ADD60E4B9AACFCAE779E0114F7",1)</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="S3" s="3">
-        <v>4</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>6</v>
+      <c r="G21" s="15" t="str">
+        <f t="shared" si="7"/>
+        <v>=DISPIMG("ID_D7722B57E05447DEBE72C39EE8A9F731",1)</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I21" s="17">
+        <v>2</v>
+      </c>
+      <c r="J21" s="20" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="4" ht="31" customHeight="1" spans="1:20">
-      <c r="A4" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_7BE895EBAF304A60A4C5B4F2F664E2C4",1)</f>
-        <v>=DISPIMG("ID_7BE895EBAF304A60A4C5B4F2F664E2C4",1)</v>
-      </c>
-      <c r="B4" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_0DCABE9F44DA4E239F21ECDEB726BF58",1)</f>
-        <v>=DISPIMG("ID_0DCABE9F44DA4E239F21ECDEB726BF58",1)</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3">
-        <v>3</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_57DECDAF621B4ABDBC7D8E64B2E10BEC",1)</f>
-        <v>=DISPIMG("ID_57DECDAF621B4ABDBC7D8E64B2E10BEC",1)</v>
-      </c>
-      <c r="G4" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_7E54EC765F954BF0BF6E3014289FAE84",1)</f>
-        <v>=DISPIMG("ID_7E54EC765F954BF0BF6E3014289FAE84",1)</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_950575228AB54565B95BE1A8CDDED0CF",1)</f>
-        <v>=DISPIMG("ID_950575228AB54565B95BE1A8CDDED0CF",1)</v>
-      </c>
-      <c r="L4" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_1F0BE2047E2A4BAEAD892BAD47B3B5A6",1)</f>
-        <v>=DISPIMG("ID_1F0BE2047E2A4BAEAD892BAD47B3B5A6",1)</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N4" s="3">
-        <v>3</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="P4" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</f>
-        <v>=DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</v>
-      </c>
-      <c r="Q4" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_A78947ADD60E4B9AACFCAE779E0114F7",1)</f>
-        <v>=DISPIMG("ID_A78947ADD60E4B9AACFCAE779E0114F7",1)</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="S4" s="3">
-        <v>4</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" ht="31" customHeight="1" spans="1:20">
-      <c r="A5" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_F2534797B2514259B37B3F90C14104CE",1)</f>
-        <v>=DISPIMG("ID_F2534797B2514259B37B3F90C14104CE",1)</v>
-      </c>
-      <c r="B5" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_0DCABE9F44DA4E239F21ECDEB726BF58",1)</f>
-        <v>=DISPIMG("ID_0DCABE9F44DA4E239F21ECDEB726BF58",1)</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_BA2487D371F2480A955BB261416FB890",1)</f>
-        <v>=DISPIMG("ID_BA2487D371F2480A955BB261416FB890",1)</v>
-      </c>
-      <c r="G5" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_7E54EC765F954BF0BF6E3014289FAE84",1)</f>
-        <v>=DISPIMG("ID_7E54EC765F954BF0BF6E3014289FAE84",1)</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_950575228AB54565B95BE1A8CDDED0CF",1)</f>
-        <v>=DISPIMG("ID_950575228AB54565B95BE1A8CDDED0CF",1)</v>
-      </c>
-      <c r="L5" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_1F0BE2047E2A4BAEAD892BAD47B3B5A6",1)</f>
-        <v>=DISPIMG("ID_1F0BE2047E2A4BAEAD892BAD47B3B5A6",1)</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="3">
-        <v>5</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P5" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</f>
-        <v>=DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</v>
-      </c>
-      <c r="Q5" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_A78947ADD60E4B9AACFCAE779E0114F7",1)</f>
-        <v>=DISPIMG("ID_A78947ADD60E4B9AACFCAE779E0114F7",1)</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="S5" s="3">
-        <v>4</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" ht="31" customHeight="1" spans="1:20">
-      <c r="A6" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_BA2487D371F2480A955BB261416FB890",1)</f>
-        <v>=DISPIMG("ID_BA2487D371F2480A955BB261416FB890",1)</v>
-      </c>
-      <c r="B6" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_0DCABE9F44DA4E239F21ECDEB726BF58",1)</f>
-        <v>=DISPIMG("ID_0DCABE9F44DA4E239F21ECDEB726BF58",1)</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="3">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_9A490142D9BF4C41BEA4AF01A76599D2",1)</f>
-        <v>=DISPIMG("ID_9A490142D9BF4C41BEA4AF01A76599D2",1)</v>
-      </c>
-      <c r="G6" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_7E54EC765F954BF0BF6E3014289FAE84",1)</f>
-        <v>=DISPIMG("ID_7E54EC765F954BF0BF6E3014289FAE84",1)</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_950575228AB54565B95BE1A8CDDED0CF",1)</f>
-        <v>=DISPIMG("ID_950575228AB54565B95BE1A8CDDED0CF",1)</v>
-      </c>
-      <c r="L6" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_1F0BE2047E2A4BAEAD892BAD47B3B5A6",1)</f>
-        <v>=DISPIMG("ID_1F0BE2047E2A4BAEAD892BAD47B3B5A6",1)</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N6" s="3">
-        <v>0</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P6" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</f>
-        <v>=DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</v>
-      </c>
-      <c r="Q6" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_A78947ADD60E4B9AACFCAE779E0114F7",1)</f>
-        <v>=DISPIMG("ID_A78947ADD60E4B9AACFCAE779E0114F7",1)</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S6" s="3">
-        <v>4</v>
-      </c>
-      <c r="T6" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" ht="31" customHeight="1" spans="1:20">
-      <c r="A7" s="1" t="str">
-        <f t="shared" ref="A7:A11" si="0">_xlfn.DISPIMG("ID_268B8A0A44544341B29F9DDA7FA1D51C",1)</f>
-        <v>=DISPIMG("ID_268B8A0A44544341B29F9DDA7FA1D51C",1)</v>
-      </c>
-      <c r="B7" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</f>
-        <v>=DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="3">
-        <v>6</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_ED6C9EB4D46D47A0B011F533288D71BF",1)</f>
-        <v>=DISPIMG("ID_ED6C9EB4D46D47A0B011F533288D71BF",1)</v>
-      </c>
-      <c r="G7" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</f>
-        <v>=DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="3">
-        <v>1</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="1" t="str">
-        <f t="shared" ref="K7:K11" si="1">_xlfn.DISPIMG("ID_AE82F2EF4A454B3CBA695725E1E9B708",1)</f>
-        <v>=DISPIMG("ID_AE82F2EF4A454B3CBA695725E1E9B708",1)</v>
-      </c>
-      <c r="L7" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_1A3A7A7BDCEE4A4E81B55D77328F65F8",1)</f>
-        <v>=DISPIMG("ID_1A3A7A7BDCEE4A4E81B55D77328F65F8",1)</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N7" s="3">
-        <v>4</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="P7" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</f>
-        <v>=DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</v>
-      </c>
-      <c r="Q7" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_D7722B57E05447DEBE72C39EE8A9F731",1)</f>
-        <v>=DISPIMG("ID_D7722B57E05447DEBE72C39EE8A9F731",1)</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S7" s="3">
-        <v>2</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" ht="31" customHeight="1" spans="1:20">
-      <c r="A8" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_6000619F3E9D44F6AE6CD3C3E56CAD75",1)</f>
-        <v>=DISPIMG("ID_6000619F3E9D44F6AE6CD3C3E56CAD75",1)</v>
-      </c>
-      <c r="B8" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</f>
-        <v>=DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="3">
-        <v>6</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_58AD4992DB3B48FC91CB1DC9640F186D",1)</f>
-        <v>=DISPIMG("ID_58AD4992DB3B48FC91CB1DC9640F186D",1)</v>
-      </c>
-      <c r="G8" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</f>
-        <v>=DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>=DISPIMG("ID_AE82F2EF4A454B3CBA695725E1E9B708",1)</v>
-      </c>
-      <c r="L8" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_1A3A7A7BDCEE4A4E81B55D77328F65F8",1)</f>
-        <v>=DISPIMG("ID_1A3A7A7BDCEE4A4E81B55D77328F65F8",1)</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N8" s="3">
-        <v>4</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="P8" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_6FD6430484BB49FE9601020DAB644F5B",1)</f>
-        <v>=DISPIMG("ID_6FD6430484BB49FE9601020DAB644F5B",1)</v>
-      </c>
-      <c r="Q8" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_D7722B57E05447DEBE72C39EE8A9F731",1)</f>
-        <v>=DISPIMG("ID_D7722B57E05447DEBE72C39EE8A9F731",1)</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="S8" s="3">
-        <v>2</v>
-      </c>
-      <c r="T8" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" ht="31" customHeight="1" spans="1:20">
-      <c r="A9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>=DISPIMG("ID_268B8A0A44544341B29F9DDA7FA1D51C",1)</v>
-      </c>
-      <c r="B9" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</f>
-        <v>=DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="3">
-        <v>4</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_ED6C9EB4D46D47A0B011F533288D71BF",1)</f>
-        <v>=DISPIMG("ID_ED6C9EB4D46D47A0B011F533288D71BF",1)</v>
-      </c>
-      <c r="G9" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</f>
-        <v>=DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_58917936AC9A4E2E89C66D86230F0730",1)</f>
-        <v>=DISPIMG("ID_58917936AC9A4E2E89C66D86230F0730",1)</v>
-      </c>
-      <c r="L9" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_1A3A7A7BDCEE4A4E81B55D77328F65F8",1)</f>
-        <v>=DISPIMG("ID_1A3A7A7BDCEE4A4E81B55D77328F65F8",1)</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="N9" s="3">
-        <v>4</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="P9" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</f>
-        <v>=DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</v>
-      </c>
-      <c r="Q9" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_D7722B57E05447DEBE72C39EE8A9F731",1)</f>
-        <v>=DISPIMG("ID_D7722B57E05447DEBE72C39EE8A9F731",1)</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="S9" s="3">
-        <v>1</v>
-      </c>
-      <c r="T9" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" ht="31" customHeight="1" spans="1:20">
-      <c r="A10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>=DISPIMG("ID_268B8A0A44544341B29F9DDA7FA1D51C",1)</v>
-      </c>
-      <c r="B10" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</f>
-        <v>=DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="3">
-        <v>4</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_959C3ED946B741B495F5F344457CA70A",1)</f>
-        <v>=DISPIMG("ID_959C3ED946B741B495F5F344457CA70A",1)</v>
-      </c>
-      <c r="G10" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</f>
-        <v>=DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_AE2522B87EF74B1095DD7DEA2A944CB0",1)</f>
-        <v>=DISPIMG("ID_AE2522B87EF74B1095DD7DEA2A944CB0",1)</v>
-      </c>
-      <c r="L10" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_1A3A7A7BDCEE4A4E81B55D77328F65F8",1)</f>
-        <v>=DISPIMG("ID_1A3A7A7BDCEE4A4E81B55D77328F65F8",1)</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="N10" s="3">
-        <v>1</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="P10" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_115E27EB0FD249CAB22FFC543F696862",1)</f>
-        <v>=DISPIMG("ID_115E27EB0FD249CAB22FFC543F696862",1)</v>
-      </c>
-      <c r="Q10" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_D7722B57E05447DEBE72C39EE8A9F731",1)</f>
-        <v>=DISPIMG("ID_D7722B57E05447DEBE72C39EE8A9F731",1)</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="S10" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="T10" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" ht="31" customHeight="1" spans="1:20">
-      <c r="A11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>=DISPIMG("ID_268B8A0A44544341B29F9DDA7FA1D51C",1)</v>
-      </c>
-      <c r="B11" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</f>
-        <v>=DISPIMG("ID_B38396FE47394E2C8C4216DAB3EEFA09",1)</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="3">
-        <v>3</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_6BF2B7BDCEC143CB9B923DEF2ED950E0",1)</f>
-        <v>=DISPIMG("ID_6BF2B7BDCEC143CB9B923DEF2ED950E0",1)</v>
-      </c>
-      <c r="G11" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</f>
-        <v>=DISPIMG("ID_4AF1644E23F5469C8427DD1B1F10A83E",1)</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>=DISPIMG("ID_AE82F2EF4A454B3CBA695725E1E9B708",1)</v>
-      </c>
-      <c r="L11" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_1A3A7A7BDCEE4A4E81B55D77328F65F8",1)</f>
-        <v>=DISPIMG("ID_1A3A7A7BDCEE4A4E81B55D77328F65F8",1)</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="N11" s="3">
-        <v>1</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="P11" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</f>
-        <v>=DISPIMG("ID_E90DCBB78AAB4DD2A719460C116F281B",1)</v>
-      </c>
-      <c r="Q11" s="1" t="str">
-        <f>_xlfn.DISPIMG("ID_D7722B57E05447DEBE72C39EE8A9F731",1)</f>
-        <v>=DISPIMG("ID_D7722B57E05447DEBE72C39EE8A9F731",1)</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="S11" s="3">
-        <v>2</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" ht="31" customHeight="1" spans="4:19">
-      <c r="D12" s="7">
-        <f>SUM(D2:D11)</f>
-        <v>34</v>
-      </c>
-      <c r="I12" s="7">
-        <f>SUM(I2:I11)</f>
-        <v>5</v>
-      </c>
-      <c r="N12" s="7">
-        <f>SUM(N2:N11)</f>
-        <v>26</v>
-      </c>
-      <c r="S12" s="7">
-        <f>SUM(S2:S11)</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" ht="31" customHeight="1"/>
-    <row r="14" ht="31" customHeight="1"/>
-    <row r="15" ht="31" customHeight="1"/>
-    <row r="16" ht="31" customHeight="1"/>
   </sheetData>
+  <conditionalFormatting sqref="I1">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="8" tint="0.8"/>
+        <color theme="8"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N1">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="8" tint="0.8"/>
+        <color theme="8"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S1">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="8" tint="0.8"/>
+        <color theme="8"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E2">
+    <cfRule type="containsText" dxfId="0" priority="43" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2">
+    <cfRule type="containsText" dxfId="0" priority="50" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",O2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T2">
+    <cfRule type="containsText" dxfId="0" priority="92" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",T2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3">
+    <cfRule type="containsText" dxfId="0" priority="45" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",J3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3">
+    <cfRule type="containsText" dxfId="0" priority="51" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",O3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T3">
+    <cfRule type="containsText" dxfId="0" priority="57" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",T3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O4">
+    <cfRule type="containsText" dxfId="0" priority="97" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",O4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T4">
+    <cfRule type="containsText" dxfId="0" priority="56" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",T4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="containsText" dxfId="0" priority="67" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",E5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O5">
+    <cfRule type="containsText" dxfId="0" priority="52" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",O5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T5">
+    <cfRule type="containsText" dxfId="0" priority="55" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",T5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="containsText" dxfId="0" priority="42" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",E6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O6">
+    <cfRule type="containsText" dxfId="0" priority="74" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",O6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T6">
+    <cfRule type="containsText" dxfId="0" priority="54" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",T6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7">
+    <cfRule type="containsText" dxfId="0" priority="44" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",J7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O7">
+    <cfRule type="containsText" dxfId="0" priority="96" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",O7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T7">
+    <cfRule type="containsText" dxfId="0" priority="49" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",T7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O8">
+    <cfRule type="containsText" dxfId="0" priority="95" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",O8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T8">
+    <cfRule type="containsText" dxfId="0" priority="48" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",T8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="containsText" dxfId="0" priority="60" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",E9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O9">
+    <cfRule type="containsText" dxfId="0" priority="94" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",O9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T9">
+    <cfRule type="containsText" dxfId="0" priority="47" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",T9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="containsText" dxfId="0" priority="59" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",E10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O10">
+    <cfRule type="containsText" dxfId="0" priority="93" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",O10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T10">
+    <cfRule type="containsText" dxfId="0" priority="62" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",T10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="containsText" dxfId="0" priority="58" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",E11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O11">
+    <cfRule type="containsText" dxfId="0" priority="53" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",O11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T11">
+    <cfRule type="containsText" dxfId="0" priority="46" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",T11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="containsText" dxfId="0" priority="9" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",E12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J12">
+    <cfRule type="containsText" dxfId="0" priority="19" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",J12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N12">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="8" tint="0.8"/>
+        <color theme="8"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S12">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="8" tint="0.8"/>
+        <color theme="8"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="containsText" dxfId="0" priority="10" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",E13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13">
+    <cfRule type="containsText" dxfId="0" priority="16" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",J13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="containsText" dxfId="0" priority="24" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",E14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J14">
     <cfRule type="containsText" dxfId="0" priority="15" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",E2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O2">
+      <formula>NOT(ISERROR(SEARCH("1st",J14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="containsText" dxfId="0" priority="11" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",E15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15">
+    <cfRule type="containsText" dxfId="0" priority="14" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",J15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="containsText" dxfId="0" priority="18" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",E16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16">
+    <cfRule type="containsText" dxfId="0" priority="13" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",J16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
+    <cfRule type="containsText" dxfId="0" priority="23" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",E17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17">
+    <cfRule type="containsText" dxfId="0" priority="8" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",J17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18">
     <cfRule type="containsText" dxfId="0" priority="22" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",O2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T2">
-    <cfRule type="containsText" dxfId="0" priority="64" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",T2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3">
+      <formula>NOT(ISERROR(SEARCH("1st",E18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J18">
+    <cfRule type="containsText" dxfId="0" priority="7" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",J18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="containsText" dxfId="0" priority="21" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",E19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J19">
+    <cfRule type="containsText" dxfId="0" priority="6" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",J19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20">
+    <cfRule type="containsText" dxfId="0" priority="20" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",E20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J20">
     <cfRule type="containsText" dxfId="0" priority="17" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",J3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O3">
-    <cfRule type="containsText" dxfId="0" priority="23" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",O3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T3">
-    <cfRule type="containsText" dxfId="0" priority="29" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",T3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O4">
-    <cfRule type="containsText" dxfId="0" priority="69" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",O4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T4">
-    <cfRule type="containsText" dxfId="0" priority="28" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",T4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="0" priority="39" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",E5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O5">
-    <cfRule type="containsText" dxfId="0" priority="24" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",O5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T5">
-    <cfRule type="containsText" dxfId="0" priority="27" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",T5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="0" priority="14" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",E6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O6">
-    <cfRule type="containsText" dxfId="0" priority="46" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",O6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T6">
-    <cfRule type="containsText" dxfId="0" priority="26" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",T6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J7">
-    <cfRule type="containsText" dxfId="0" priority="16" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",J7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O7">
-    <cfRule type="containsText" dxfId="0" priority="68" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",O7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T7">
-    <cfRule type="containsText" dxfId="0" priority="21" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",T7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O8">
-    <cfRule type="containsText" dxfId="0" priority="67" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",O8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T8">
-    <cfRule type="containsText" dxfId="0" priority="20" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",T8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="0" priority="32" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",E9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O9">
-    <cfRule type="containsText" dxfId="0" priority="66" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",O9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T9">
-    <cfRule type="containsText" dxfId="0" priority="19" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",T9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
-    <cfRule type="containsText" dxfId="0" priority="31" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",E10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O10">
-    <cfRule type="containsText" dxfId="0" priority="65" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",O10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T10">
-    <cfRule type="containsText" dxfId="0" priority="34" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",T10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
-    <cfRule type="containsText" dxfId="0" priority="30" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",E11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O11">
-    <cfRule type="containsText" dxfId="0" priority="25" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",O11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T11">
-    <cfRule type="containsText" dxfId="0" priority="18" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",T11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
+      <formula>NOT(ISERROR(SEARCH("1st",J20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
+    <cfRule type="containsText" dxfId="0" priority="12" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",E21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J21">
+    <cfRule type="containsText" dxfId="0" priority="5" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",J21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:D21">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3084,7 +3464,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
+  <conditionalFormatting sqref="I12:I21">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3094,8 +3474,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N12">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="D1:D11 D23:D1048576">
+    <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3104,8 +3484,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S12">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="I2:I11 I23:I1048576">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3114,8 +3494,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D11 D13:D1048576">
-    <cfRule type="colorScale" priority="11">
+  <conditionalFormatting sqref="J2 J4:J6 J8:J11">
+    <cfRule type="containsText" dxfId="0" priority="76" operator="between" text="1st">
+      <formula>NOT(ISERROR(SEARCH("1st",J2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N11 N13:N1048576">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3124,8 +3509,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I11 I13:I1048576">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="S2:S11 S13:S1048576">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3134,31 +3519,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N11 N13:N1048576">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="8" tint="0.8"/>
-        <color theme="8"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S1:S11 S13:S1048576">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="8" tint="0.8"/>
-        <color theme="8"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J2 J4:J6 J8:J11">
-    <cfRule type="containsText" dxfId="0" priority="48" operator="between" text="1st">
-      <formula>NOT(ISERROR(SEARCH("1st",J2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>